<commit_message>
Alterando a caminho das planilhas
</commit_message>
<xml_diff>
--- a/data_sources/Setembro/amil_header_bronze.xlsx
+++ b/data_sources/Setembro/amil_header_bronze.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DomRock\FATEC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF373F26-5746-4A85-9CE2-08245A867C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="affix_amil_header_bronze (2)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'affix_amil_header_bronze (2)'!$A$1:$E$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'affix_amil_header_bronze (2)'!$A$1:$F$588</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="109">
   <si>
     <t>_idFile</t>
   </si>
@@ -347,13 +341,16 @@
   </si>
   <si>
     <t>632ca7ffa80e50e9252585f6</t>
+  </si>
+  <si>
+    <t>_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,8 +485,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,6 +672,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF70AD47"/>
       </patternFill>
     </fill>
   </fills>
@@ -830,8 +841,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -863,10 +876,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1179,1749 +1192,1773 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
       <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>933510000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>43708021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
       <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
         <v>722777000</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>43708018</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>722771000</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>43708020</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
       <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>1190478000</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>43778802</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
         <v>1189426000</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
         <v>43762485</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>1189447000</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
         <v>43778801</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
       <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>1189426000</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
         <v>43762485</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>1189447000</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
         <v>43778801</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
       <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>1189426000</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
         <v>43762485</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
       <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
         <v>1191014000</v>
       </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
         <v>43761551</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
       <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
         <v>1584460000</v>
       </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12">
         <v>43762494</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
       <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
         <v>1190474000</v>
       </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13">
         <v>43778739</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
       <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
         <v>1191011000</v>
       </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14">
         <v>43761669</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
       <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
         <v>1190477000</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15">
         <v>43761917</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
       <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>1264565000</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16">
         <v>43762369</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
       <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
         <v>1189449000</v>
       </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
         <v>43761736</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
       <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
         <v>1345942000</v>
       </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18">
         <v>43762015</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
       <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
         <v>1201393000</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19">
         <v>43761817</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
       <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
         <v>1189455000</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
         <v>43762154</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
       <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
         <v>1275924000</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21">
         <v>43761994</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
       <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
         <v>1696455000</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22">
         <v>43762589</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
       <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
         <v>1697090000</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23">
         <v>43762502</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
       <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
         <v>1584435000</v>
       </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24">
         <v>43761725</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
       <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
         <v>310426000</v>
       </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25">
         <v>43762726</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
       <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
         <v>1263389000</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26">
         <v>43762362</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
       <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
         <v>1682027000</v>
       </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27">
         <v>43761800</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
       <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
         <v>108697000</v>
       </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28">
         <v>43762563</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>34</v>
       </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
       <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
         <v>1697084000</v>
       </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29">
         <v>43761524</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
       <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
         <v>1217130000</v>
       </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30">
         <v>43761916</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
       <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
         <v>189733000</v>
       </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31">
         <v>43762582</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
       <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
         <v>310572000</v>
       </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32">
         <v>43762018</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>38</v>
       </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
       <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
         <v>1221498000</v>
       </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33">
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
         <v>43762283</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
       <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
         <v>311084000</v>
       </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34">
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34">
         <v>1119216</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
       <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
         <v>927223000</v>
       </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35">
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35">
         <v>43762172</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
       <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
         <v>927616000</v>
       </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36">
         <v>43761664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
       <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
         <v>1189445000</v>
       </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37">
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37">
         <v>43762028</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
       <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
         <v>318048000</v>
       </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38">
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38">
         <v>43762397</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>44</v>
       </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
       <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
         <v>1190478000</v>
       </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39">
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39">
         <v>43778802</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>45</v>
       </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
       <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
         <v>320087000</v>
       </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40">
         <v>1119230</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>46</v>
       </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
       <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
         <v>938494000</v>
       </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41">
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41">
         <v>709990</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>47</v>
       </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
       <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
         <v>927614000</v>
       </c>
-      <c r="D42" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42">
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42">
         <v>43761977</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>48</v>
       </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
       <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
         <v>722776000</v>
       </c>
-      <c r="D43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43">
         <v>44019520</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>50</v>
       </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
       <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
         <v>933509000</v>
       </c>
-      <c r="D44" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44">
         <v>44019522</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
       <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
         <v>933528000</v>
       </c>
-      <c r="D45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45">
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45">
         <v>44019521</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>52</v>
       </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
       <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
         <v>1684868000</v>
       </c>
-      <c r="D46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46">
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46">
         <v>44011579</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>53</v>
       </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
       <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
         <v>1689198000</v>
       </c>
-      <c r="D47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47">
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47">
         <v>44011129</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>54</v>
       </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
       <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
         <v>1704108000</v>
       </c>
-      <c r="D48" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48">
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48">
         <v>44011556</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>55</v>
       </c>
-      <c r="B49">
-        <v>3</v>
-      </c>
       <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
         <v>1704119000</v>
       </c>
-      <c r="D49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49">
+      <c r="E49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49">
         <v>44011588</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
       <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
         <v>1704924000</v>
       </c>
-      <c r="D50" t="s">
-        <v>49</v>
-      </c>
-      <c r="E50">
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50">
         <v>44010991</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
       <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
         <v>1704926000</v>
       </c>
-      <c r="D51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51">
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51">
         <v>44010997</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>58</v>
       </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
       <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
         <v>1719634000</v>
       </c>
-      <c r="D52" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52">
+      <c r="E52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52">
         <v>44011219</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>59</v>
       </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
       <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
         <v>1728289000</v>
       </c>
-      <c r="D53" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53">
+      <c r="E53" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53">
         <v>44011248</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
       <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
         <v>1756843000</v>
       </c>
-      <c r="D54" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54">
+      <c r="E54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54">
         <v>44011244</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>61</v>
       </c>
-      <c r="B55">
-        <v>3</v>
-      </c>
       <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
         <v>108739000</v>
       </c>
-      <c r="D55" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55">
+      <c r="E55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55">
         <v>44011581</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="B56">
-        <v>3</v>
-      </c>
       <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
         <v>265529000</v>
       </c>
-      <c r="D56" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56">
+      <c r="E56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56">
         <v>44011321</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>63</v>
       </c>
-      <c r="B57">
-        <v>3</v>
-      </c>
       <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
         <v>265549000</v>
       </c>
-      <c r="D57" t="s">
-        <v>49</v>
-      </c>
-      <c r="E57">
+      <c r="E57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57">
         <v>44011483</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="B58">
-        <v>3</v>
-      </c>
       <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
         <v>310450000</v>
       </c>
-      <c r="D58" t="s">
-        <v>49</v>
-      </c>
-      <c r="E58">
+      <c r="E58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F58">
         <v>1127100</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>65</v>
       </c>
-      <c r="B59">
-        <v>3</v>
-      </c>
       <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
         <v>310453000</v>
       </c>
-      <c r="D59" t="s">
-        <v>49</v>
-      </c>
-      <c r="E59">
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59">
         <v>44011331</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>66</v>
       </c>
-      <c r="B60">
-        <v>3</v>
-      </c>
       <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
         <v>310468000</v>
       </c>
-      <c r="D60" t="s">
-        <v>49</v>
-      </c>
-      <c r="E60">
+      <c r="E60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F60">
         <v>44011033</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>67</v>
       </c>
-      <c r="B61">
-        <v>3</v>
-      </c>
       <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
         <v>310603000</v>
       </c>
-      <c r="D61" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61">
+      <c r="E61" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61">
         <v>44010684</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>68</v>
       </c>
-      <c r="B62">
-        <v>3</v>
-      </c>
       <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
         <v>326266000</v>
       </c>
-      <c r="D62" t="s">
-        <v>49</v>
-      </c>
-      <c r="E62">
+      <c r="E62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62">
         <v>44010741</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>69</v>
       </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
       <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
         <v>326288000</v>
       </c>
-      <c r="D63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E63">
+      <c r="E63" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63">
         <v>44011246</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>70</v>
       </c>
-      <c r="B64">
-        <v>3</v>
-      </c>
       <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
         <v>326300000</v>
       </c>
-      <c r="D64" t="s">
-        <v>49</v>
-      </c>
-      <c r="E64">
+      <c r="E64" t="s">
+        <v>49</v>
+      </c>
+      <c r="F64">
         <v>44010966</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>71</v>
       </c>
-      <c r="B65">
-        <v>3</v>
-      </c>
       <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
         <v>326376000</v>
       </c>
-      <c r="D65" t="s">
-        <v>49</v>
-      </c>
-      <c r="E65">
+      <c r="E65" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65">
         <v>44011644</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>72</v>
       </c>
-      <c r="B66">
-        <v>3</v>
-      </c>
       <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
         <v>342418000</v>
       </c>
-      <c r="D66" t="s">
-        <v>49</v>
-      </c>
-      <c r="E66">
+      <c r="E66" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66">
         <v>44011032</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>73</v>
       </c>
-      <c r="B67">
-        <v>3</v>
-      </c>
       <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
         <v>552068000</v>
       </c>
-      <c r="D67" t="s">
-        <v>49</v>
-      </c>
-      <c r="E67">
+      <c r="E67" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67">
         <v>44011188</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>74</v>
       </c>
-      <c r="B68">
-        <v>3</v>
-      </c>
       <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
         <v>927264000</v>
       </c>
-      <c r="D68" t="s">
-        <v>49</v>
-      </c>
-      <c r="E68">
+      <c r="E68" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68">
         <v>44011433</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>75</v>
       </c>
-      <c r="B69">
-        <v>3</v>
-      </c>
       <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
         <v>927278000</v>
       </c>
-      <c r="D69" t="s">
-        <v>49</v>
-      </c>
-      <c r="E69">
+      <c r="E69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69">
         <v>44011034</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>76</v>
       </c>
-      <c r="B70">
-        <v>3</v>
-      </c>
       <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
         <v>927627000</v>
       </c>
-      <c r="D70" t="s">
-        <v>49</v>
-      </c>
-      <c r="E70">
+      <c r="E70" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70">
         <v>44010543</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>77</v>
       </c>
-      <c r="B71">
-        <v>3</v>
-      </c>
       <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71">
         <v>927630000</v>
       </c>
-      <c r="D71" t="s">
-        <v>49</v>
-      </c>
-      <c r="E71">
+      <c r="E71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71">
         <v>44011656</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>78</v>
       </c>
-      <c r="B72">
-        <v>3</v>
-      </c>
       <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
         <v>927631000</v>
       </c>
-      <c r="D72" t="s">
-        <v>49</v>
-      </c>
-      <c r="E72">
+      <c r="E72" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72">
         <v>44011035</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>79</v>
       </c>
-      <c r="B73">
-        <v>3</v>
-      </c>
       <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
         <v>927632000</v>
       </c>
-      <c r="D73" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73">
+      <c r="E73" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73">
         <v>44010663</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>80</v>
       </c>
-      <c r="B74">
-        <v>3</v>
-      </c>
       <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
         <v>973330000</v>
       </c>
-      <c r="D74" t="s">
-        <v>49</v>
-      </c>
-      <c r="E74">
+      <c r="E74" t="s">
+        <v>49</v>
+      </c>
+      <c r="F74">
         <v>1127091</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>81</v>
       </c>
-      <c r="B75">
-        <v>3</v>
-      </c>
       <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
         <v>1195733000</v>
       </c>
-      <c r="D75" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75">
+      <c r="E75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75">
         <v>44019011</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>82</v>
       </c>
-      <c r="B76">
-        <v>3</v>
-      </c>
       <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
         <v>1195738000</v>
       </c>
-      <c r="D76" t="s">
-        <v>49</v>
-      </c>
-      <c r="E76">
+      <c r="E76" t="s">
+        <v>49</v>
+      </c>
+      <c r="F76">
         <v>44019012</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>83</v>
       </c>
-      <c r="B77">
-        <v>3</v>
-      </c>
       <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
         <v>1195750000</v>
       </c>
-      <c r="D77" t="s">
-        <v>49</v>
-      </c>
-      <c r="E77">
+      <c r="E77" t="s">
+        <v>49</v>
+      </c>
+      <c r="F77">
         <v>44010885</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>84</v>
       </c>
-      <c r="B78">
-        <v>3</v>
-      </c>
       <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
         <v>1195751000</v>
       </c>
-      <c r="D78" t="s">
-        <v>49</v>
-      </c>
-      <c r="E78">
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78">
         <v>44010647</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>85</v>
       </c>
-      <c r="B79">
-        <v>3</v>
-      </c>
       <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79">
         <v>1195752000</v>
       </c>
-      <c r="D79" t="s">
-        <v>49</v>
-      </c>
-      <c r="E79">
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79">
         <v>44011285</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>86</v>
       </c>
-      <c r="B80">
-        <v>3</v>
-      </c>
       <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
         <v>1195756000</v>
       </c>
-      <c r="D80" t="s">
-        <v>49</v>
-      </c>
-      <c r="E80">
+      <c r="E80" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80">
         <v>44011016</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>87</v>
       </c>
-      <c r="B81">
-        <v>3</v>
-      </c>
       <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81">
         <v>1195761000</v>
       </c>
-      <c r="D81" t="s">
-        <v>49</v>
-      </c>
-      <c r="E81">
+      <c r="E81" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81">
         <v>44011214</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>88</v>
       </c>
-      <c r="B82">
-        <v>3</v>
-      </c>
       <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82">
         <v>1195762000</v>
       </c>
-      <c r="D82" t="s">
-        <v>49</v>
-      </c>
-      <c r="E82">
+      <c r="E82" t="s">
+        <v>49</v>
+      </c>
+      <c r="F82">
         <v>44019000</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>89</v>
       </c>
-      <c r="B83">
-        <v>3</v>
-      </c>
       <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
         <v>1195772000</v>
       </c>
-      <c r="D83" t="s">
-        <v>49</v>
-      </c>
-      <c r="E83">
+      <c r="E83" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83">
         <v>44011149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>90</v>
       </c>
-      <c r="B84">
-        <v>3</v>
-      </c>
       <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84">
         <v>1195777000</v>
       </c>
-      <c r="D84" t="s">
-        <v>49</v>
-      </c>
-      <c r="E84">
+      <c r="E84" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84">
         <v>44011405</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>91</v>
       </c>
-      <c r="B85">
-        <v>3</v>
-      </c>
       <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
         <v>1196918000</v>
       </c>
-      <c r="D85" t="s">
-        <v>49</v>
-      </c>
-      <c r="E85">
+      <c r="E85" t="s">
+        <v>49</v>
+      </c>
+      <c r="F85">
         <v>44010793</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>92</v>
       </c>
-      <c r="B86">
-        <v>3</v>
-      </c>
       <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
         <v>1196922000</v>
       </c>
-      <c r="D86" t="s">
-        <v>49</v>
-      </c>
-      <c r="E86">
+      <c r="E86" t="s">
+        <v>49</v>
+      </c>
+      <c r="F86">
         <v>44011017</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>93</v>
       </c>
-      <c r="B87">
-        <v>3</v>
-      </c>
       <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
         <v>1197772000</v>
       </c>
-      <c r="D87" t="s">
-        <v>49</v>
-      </c>
-      <c r="E87">
+      <c r="E87" t="s">
+        <v>49</v>
+      </c>
+      <c r="F87">
         <v>44018973</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>94</v>
       </c>
-      <c r="B88">
-        <v>3</v>
-      </c>
       <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
         <v>1197781000</v>
       </c>
-      <c r="D88" t="s">
-        <v>49</v>
-      </c>
-      <c r="E88">
+      <c r="E88" t="s">
+        <v>49</v>
+      </c>
+      <c r="F88">
         <v>44011061</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>95</v>
       </c>
-      <c r="B89">
-        <v>3</v>
-      </c>
       <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89">
         <v>1198437000</v>
       </c>
-      <c r="D89" t="s">
-        <v>49</v>
-      </c>
-      <c r="E89">
+      <c r="E89" t="s">
+        <v>49</v>
+      </c>
+      <c r="F89">
         <v>44011360</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>96</v>
       </c>
-      <c r="B90">
-        <v>3</v>
-      </c>
       <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
         <v>1198444000</v>
       </c>
-      <c r="D90" t="s">
-        <v>49</v>
-      </c>
-      <c r="E90">
+      <c r="E90" t="s">
+        <v>49</v>
+      </c>
+      <c r="F90">
         <v>44018950</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>97</v>
       </c>
-      <c r="B91">
-        <v>3</v>
-      </c>
       <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
         <v>1198447000</v>
       </c>
-      <c r="D91" t="s">
-        <v>49</v>
-      </c>
-      <c r="E91">
+      <c r="E91" t="s">
+        <v>49</v>
+      </c>
+      <c r="F91">
         <v>43916058</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>98</v>
       </c>
-      <c r="B92">
-        <v>3</v>
-      </c>
       <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92">
         <v>1198467000</v>
       </c>
-      <c r="D92" t="s">
-        <v>49</v>
-      </c>
-      <c r="E92">
+      <c r="E92" t="s">
+        <v>49</v>
+      </c>
+      <c r="F92">
         <v>44011679</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>99</v>
       </c>
-      <c r="B93">
-        <v>3</v>
-      </c>
       <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93">
         <v>1208895000</v>
       </c>
-      <c r="D93" t="s">
-        <v>49</v>
-      </c>
-      <c r="E93">
+      <c r="E93" t="s">
+        <v>49</v>
+      </c>
+      <c r="F93">
         <v>44011077</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>100</v>
       </c>
-      <c r="B94">
-        <v>3</v>
-      </c>
       <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94">
         <v>1208900000</v>
       </c>
-      <c r="D94" t="s">
-        <v>49</v>
-      </c>
-      <c r="E94">
+      <c r="E94" t="s">
+        <v>49</v>
+      </c>
+      <c r="F94">
         <v>44010961</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>101</v>
       </c>
-      <c r="B95">
-        <v>3</v>
-      </c>
       <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
         <v>1208911000</v>
       </c>
-      <c r="D95" t="s">
-        <v>49</v>
-      </c>
-      <c r="E95">
+      <c r="E95" t="s">
+        <v>49</v>
+      </c>
+      <c r="F95">
         <v>44011388</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>102</v>
       </c>
-      <c r="B96">
-        <v>3</v>
-      </c>
       <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
         <v>1221486000</v>
       </c>
-      <c r="D96" t="s">
-        <v>49</v>
-      </c>
-      <c r="E96">
+      <c r="E96" t="s">
+        <v>49</v>
+      </c>
+      <c r="F96">
         <v>44010650</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>103</v>
       </c>
-      <c r="B97">
-        <v>3</v>
-      </c>
       <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97">
         <v>1222713000</v>
       </c>
-      <c r="D97" t="s">
-        <v>49</v>
-      </c>
-      <c r="E97">
+      <c r="E97" t="s">
+        <v>49</v>
+      </c>
+      <c r="F97">
         <v>44010837</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>104</v>
       </c>
-      <c r="B98">
-        <v>3</v>
-      </c>
       <c r="C98">
+        <v>3</v>
+      </c>
+      <c r="D98">
         <v>1236112000</v>
       </c>
-      <c r="D98" t="s">
-        <v>49</v>
-      </c>
-      <c r="E98">
+      <c r="E98" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98">
         <v>44011218</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>105</v>
       </c>
-      <c r="B99">
-        <v>3</v>
-      </c>
       <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99">
         <v>1256423000</v>
       </c>
-      <c r="D99" t="s">
-        <v>49</v>
-      </c>
-      <c r="E99">
+      <c r="E99" t="s">
+        <v>49</v>
+      </c>
+      <c r="F99">
         <v>44011286</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>106</v>
       </c>
-      <c r="B100">
-        <v>3</v>
-      </c>
       <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100">
         <v>1279435000</v>
       </c>
-      <c r="D100" t="s">
-        <v>49</v>
-      </c>
-      <c r="E100">
+      <c r="E100" t="s">
+        <v>49</v>
+      </c>
+      <c r="F100">
         <v>44018946</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>107</v>
       </c>
-      <c r="B101">
-        <v>3</v>
-      </c>
       <c r="C101">
+        <v>3</v>
+      </c>
+      <c r="D101">
         <v>1237303000</v>
       </c>
-      <c r="D101" t="s">
-        <v>49</v>
-      </c>
-      <c r="E101">
+      <c r="E101" t="s">
+        <v>49</v>
+      </c>
+      <c r="F101">
         <v>44011284</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F588"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3129,13 +3166,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7758520-6349-490D-94F2-304053C9AA5A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{286C9F79-FEC8-4DF2-8714-B03AEDCCE390}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E12D4D58-B210-4DE1-A7A5-15148149561A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990F673D-8940-4246-B289-9A67B668644C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F7B514-3BC8-467B-AC51-B5C398F2AD55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B878BE47-B67E-4CC7-B8EE-8FCA478C3403}"/>
 </file>
</xml_diff>